<commit_message>
Cập nhật khách hàng và sửa lại thêm khách hàng trong bán hàng
</commit_message>
<xml_diff>
--- a/Nhom8_QuanLyCuaHangLaptop.xlsx
+++ b/Nhom8_QuanLyCuaHangLaptop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7650" firstSheet="1"/>
+    <workbookView windowWidth="19635" windowHeight="7650" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MoTaChucNang" sheetId="2" r:id="rId1"/>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Thống kê tình hình kinh doanh trong một </t>
     </r>
     <r>
@@ -253,6 +259,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Thống kê sản phẩm bán chạy theo </t>
     </r>
     <r>
@@ -1341,7 +1353,7 @@
     <t>Vũ Trung Kiên</t>
   </si>
   <si>
-    <t>Lê Gia Tính</t>
+    <t>Lưu Gia Tính</t>
   </si>
   <si>
     <t>Vũ Mạnh Tuấn</t>
@@ -5587,7 +5599,7 @@
   <sheetPr/>
   <dimension ref="A2:P241"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="B26" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="B26" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -8329,8 +8341,8 @@
   <sheetPr/>
   <dimension ref="A1:AD1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="Z24" sqref="Z24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G15" workbookViewId="0">
+      <selection activeCell="AB35" sqref="AB35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2166666666667" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Update gì quên rồi
</commit_message>
<xml_diff>
--- a/Nhom8_QuanLyCuaHangLaptop.xlsx
+++ b/Nhom8_QuanLyCuaHangLaptop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7650" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="19635" windowHeight="7650" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MoTaChucNang" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="356">
   <si>
     <t>DANH SÁCH MÔ TẢ CÁC CHỨC NĂNG CỦA PHẦN MỀM QUẢN LÝ CỬA HÀNG BÁN LAPTOP</t>
   </si>
@@ -997,7 +997,7 @@
     <t>Major Tasks</t>
   </si>
   <si>
-    <t>Project Completed By: 3/11/2023</t>
+    <t>Project Completed By: 29/11/2023</t>
   </si>
   <si>
     <t>Owner</t>
@@ -4754,7 +4754,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>635</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4766,21 +4766,22 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="D:\Study_In_University\nam3\HocKy1\CongNghePhanMem\DoAN\Diagram\UseCase\HoaDon.pngHoaDon"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
+        <a:srcRect t="5015" b="5015"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="7962900"/>
-          <a:ext cx="10048875" cy="6896100"/>
+          <a:off x="635" y="7962900"/>
+          <a:ext cx="10048240" cy="6896100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4796,33 +4797,34 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>635</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>180340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>125</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>151765</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="D:\Study_In_University\nam3\HocKy1\CongNghePhanMem\DoAN\Diagram\UseCase\NhapHang.pngNhapHang"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId2"/>
+        <a:srcRect l="-3" t="4004" r="3" b="3988"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="15382875"/>
-          <a:ext cx="10325100" cy="7391400"/>
+          <a:off x="635" y="15382240"/>
+          <a:ext cx="10324465" cy="7391400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4922,33 +4924,34 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>635</xdr:colOff>
       <xdr:row>202</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>199390</xdr:colOff>
       <xdr:row>238</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5" descr="D:\Study_In_University\nam3\HocKy1\CongNghePhanMem\DoAN\Diagram\UseCase\BaoCao (1).vpd.pngBaoCao (1).vpd"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId5"/>
+        <a:srcRect l="3214" t="-5" r="3214" b="5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="36556950"/>
-          <a:ext cx="8734425" cy="6657975"/>
+          <a:off x="635" y="36556950"/>
+          <a:ext cx="8733155" cy="6657975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5090,33 +5093,34 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>362</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>366</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>399</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>565785</xdr:colOff>
+      <xdr:row>411</xdr:row>
+      <xdr:rowOff>48895</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPr id="10" name="Picture 9" descr="D:\Study_In_University\nam3\HocKy1\CongNghePhanMem\DoAN\Diagram\UseCase\KhachHang.pngKhachHang"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId9"/>
+        <a:srcRect l="8401" t="4" r="8396" b="-4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="65512950"/>
-          <a:ext cx="9563100" cy="6791325"/>
+          <a:off x="9525" y="66286380"/>
+          <a:ext cx="8481060" cy="8143240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6743,7 +6747,7 @@
   <sheetPr/>
   <dimension ref="A2:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A135" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A135" workbookViewId="0">
       <selection activeCell="L142" sqref="L142"/>
     </sheetView>
   </sheetViews>
@@ -8010,8 +8014,8 @@
   <sheetPr/>
   <dimension ref="A1:AD1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G15" workbookViewId="0">
-      <selection activeCell="AB35" sqref="AB35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2166666666667" defaultRowHeight="15" customHeight="1"/>
@@ -9066,21 +9070,13 @@
         <v>277</v>
       </c>
       <c r="S24" s="140"/>
-      <c r="T24" s="141" t="s">
+      <c r="T24" s="141"/>
+      <c r="U24" s="142"/>
+      <c r="V24" s="142" t="s">
         <v>278</v>
       </c>
-      <c r="U24" s="142" t="s">
-        <v>279</v>
-      </c>
-      <c r="V24" s="142" t="s">
-        <v>279</v>
-      </c>
-      <c r="W24" s="143" t="s">
-        <v>279</v>
-      </c>
-      <c r="X24" s="143" t="s">
-        <v>279</v>
-      </c>
+      <c r="W24" s="143"/>
+      <c r="X24" s="143"/>
       <c r="Y24" s="182" t="s">
         <v>279</v>
       </c>
@@ -17107,8 +17103,8 @@
   <sheetPr/>
   <dimension ref="A2:A362"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T70" sqref="T70"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A357" workbookViewId="0">
+      <selection activeCell="P363" sqref="P363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="14.25"/>

</xml_diff>